<commit_message>
Update code table loading per recent db refactorings
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Facility" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="AgencyType" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="BedType" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="BehavioralHealthType" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="BehavioralHealthDiagnosisType" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="BondType" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="CaseStatusType" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="ChargeType" sheetId="7" state="visible" r:id="rId7"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t xml:space="preserve">FacilityID</t>
   </si>
@@ -51,9 +51,6 @@
     <t xml:space="preserve">Facility 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Facility 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">AgencyTypeID</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
     <t xml:space="preserve">AgencyType 4</t>
   </si>
   <si>
+    <t xml:space="preserve">AgencyType 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">BedTypeID</t>
   </si>
   <si>
@@ -84,46 +84,52 @@
     <t xml:space="preserve">BedType 2</t>
   </si>
   <si>
-    <t xml:space="preserve">BehavioralHealthTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthType 12</t>
+    <t xml:space="preserve">BedType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisTypeDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisType 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BehavioralHealthDiagnosisType 9</t>
   </si>
   <si>
     <t xml:space="preserve">BondTypeID</t>
@@ -135,33 +141,6 @@
     <t xml:space="preserve">BondType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">BondType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 10</t>
-  </si>
-  <si>
     <t xml:space="preserve">CaseStatusTypeID</t>
   </si>
   <si>
@@ -171,6 +150,24 @@
     <t xml:space="preserve">CaseStatusType 1</t>
   </si>
   <si>
+    <t xml:space="preserve">CaseStatusType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaseStatusType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaseStatusType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaseStatusType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaseStatusType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaseStatusType 7</t>
+  </si>
+  <si>
     <t xml:space="preserve">ChargeTypeID</t>
   </si>
   <si>
@@ -180,6 +177,27 @@
     <t xml:space="preserve">ChargeType 1</t>
   </si>
   <si>
+    <t xml:space="preserve">ChargeType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 8</t>
+  </si>
+  <si>
     <t xml:space="preserve">EducationLevelTypeID</t>
   </si>
   <si>
@@ -219,9 +237,6 @@
     <t xml:space="preserve">EducationLevelType 11</t>
   </si>
   <si>
-    <t xml:space="preserve">EducationLevelType 12</t>
-  </si>
-  <si>
     <t xml:space="preserve">HousingStatusTypeID</t>
   </si>
   <si>
@@ -246,6 +261,18 @@
     <t xml:space="preserve">HousingStatusType 6</t>
   </si>
   <si>
+    <t xml:space="preserve">HousingStatusType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HousingStatusType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HousingStatusType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HousingStatusType 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">IncomeLevelTypeID</t>
   </si>
   <si>
@@ -258,33 +285,6 @@
     <t xml:space="preserve">IncomeLevelType 2</t>
   </si>
   <si>
-    <t xml:space="preserve">IncomeLevelType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IncomeLevelType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IncomeLevelType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IncomeLevelType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IncomeLevelType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IncomeLevelType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IncomeLevelType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IncomeLevelType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IncomeLevelType 11</t>
-  </si>
-  <si>
     <t xml:space="preserve">JurisdictionTypeID</t>
   </si>
   <si>
@@ -312,12 +312,6 @@
     <t xml:space="preserve">JurisdictionType 7</t>
   </si>
   <si>
-    <t xml:space="preserve">JurisdictionType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JurisdictionType 9</t>
-  </si>
-  <si>
     <t xml:space="preserve">LanguageTypeID</t>
   </si>
   <si>
@@ -339,202 +333,223 @@
     <t xml:space="preserve">MedicationTypeDescription</t>
   </si>
   <si>
+    <t xml:space="preserve">Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">F</t>
   </si>
   <si>
-    <t xml:space="preserve">MedicationType 1</t>
+    <t xml:space="preserve">MedicationType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusTypeDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusType 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationTypeDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceTypeCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceTypeDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexTypeCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexTypeDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 2</t>
   </si>
   <si>
     <t xml:space="preserve">T</t>
   </si>
   <si>
-    <t xml:space="preserve">MedicationType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OccupationType 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceTypeCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 1</t>
+    <t xml:space="preserve">PersonSexType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 5</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">PersonRaceType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 3</t>
+    <t xml:space="preserve">PersonSexType 6</t>
   </si>
   <si>
     <t xml:space="preserve">E</t>
   </si>
   <si>
-    <t xml:space="preserve">PersonRaceType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexTypeCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">PersonSexType 7</t>
   </si>
   <si>
     <t xml:space="preserve">PersonSexType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 9</t>
   </si>
 </sst>
 </file>
@@ -890,7 +905,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -912,7 +927,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -924,17 +939,6 @@
       </c>
       <c r="C5" t="n">
         <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -957,10 +961,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2">
@@ -968,7 +972,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3">
@@ -976,78 +980,6 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1133,22 +1065,6 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>95</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1169,10 +1085,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2">
@@ -1180,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
@@ -1188,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1212,13 +1128,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2">
@@ -1226,10 +1142,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3">
@@ -1237,10 +1153,87 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>105</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1263,10 +1256,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
@@ -1274,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3">
@@ -1282,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4">
@@ -1290,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5">
@@ -1298,7 +1291,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
@@ -1306,7 +1299,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7">
@@ -1314,7 +1307,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8">
@@ -1322,31 +1315,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1369,10 +1338,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2">
@@ -1380,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3">
@@ -1388,7 +1357,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4">
@@ -1396,7 +1365,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
@@ -1404,7 +1373,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6">
@@ -1412,7 +1381,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7">
@@ -1420,7 +1389,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8">
@@ -1428,7 +1397,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9">
@@ -1436,7 +1405,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10">
@@ -1444,7 +1413,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11">
@@ -1452,7 +1421,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12">
@@ -1460,7 +1429,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1484,13 +1453,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2">
@@ -1498,10 +1467,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3">
@@ -1509,10 +1478,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
@@ -1520,10 +1489,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
@@ -1531,10 +1500,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6">
@@ -1542,10 +1511,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7">
@@ -1553,10 +1522,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8">
@@ -1564,10 +1533,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9">
@@ -1575,10 +1544,21 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1602,13 +1582,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2">
@@ -1616,10 +1596,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3">
@@ -1627,10 +1607,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4">
@@ -1638,10 +1618,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5">
@@ -1649,10 +1629,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6">
@@ -1660,10 +1640,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7">
@@ -1671,10 +1651,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8">
@@ -1682,10 +1662,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9">
@@ -1693,21 +1673,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C10" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1730,10 +1699,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -1741,7 +1710,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -1749,7 +1718,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -1757,7 +1726,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -1765,6 +1734,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1810,6 +1787,46 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1824,16 +1841,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="22.71" customWidth="1"/>
-    <col min="2" max="2" width="31.71" customWidth="1"/>
+    <col min="1" max="1" width="31.71" customWidth="1"/>
+    <col min="2" max="2" width="40.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
@@ -1841,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -1849,7 +1866,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -1857,7 +1874,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -1865,7 +1882,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
@@ -1873,7 +1890,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -1881,7 +1898,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
@@ -1889,7 +1906,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
@@ -1897,7 +1914,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
@@ -1905,31 +1922,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1952,10 +1945,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
@@ -1963,79 +1956,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2058,10 +1979,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -2069,7 +1990,55 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2092,10 +2061,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2">
@@ -2103,7 +2072,63 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2126,10 +2151,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
@@ -2137,7 +2162,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
@@ -2145,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
@@ -2153,7 +2178,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -2161,7 +2186,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -2169,7 +2194,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7">
@@ -2177,7 +2202,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
@@ -2185,7 +2210,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
@@ -2193,7 +2218,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10">
@@ -2201,7 +2226,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11">
@@ -2209,7 +2234,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
@@ -2217,15 +2242,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2248,10 +2265,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2">
@@ -2259,7 +2276,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
@@ -2267,7 +2284,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
@@ -2275,7 +2292,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
@@ -2283,7 +2300,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
@@ -2291,7 +2308,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
@@ -2299,7 +2316,39 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename Treatment::StartDate to TreatmentStartDate, remove Treatment::EndDate
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
@@ -30,7 +30,7 @@
     <sheet name="PersonSexType" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="ProgramEligibilityType" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="SexOffenderStatusType" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="TreatmentInitiationType" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="TreatmentAdmissionReasonType" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="TreatmentStatusType" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="WorkReleaseStatusType" sheetId="27" state="visible" r:id="rId27"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
   <si>
     <t xml:space="preserve">FacilityID</t>
   </si>
@@ -52,6 +52,15 @@
     <t xml:space="preserve">Facility 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Facility 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">EnrolledHealthcareProviderID</t>
   </si>
   <si>
@@ -82,6 +91,18 @@
     <t xml:space="preserve">EnrolledHealthcareProvider 8</t>
   </si>
   <si>
+    <t xml:space="preserve">EnrolledHealthcareProvider 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnrolledHealthcareProvider 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnrolledHealthcareProvider 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnrolledHealthcareProvider 12</t>
+  </si>
+  <si>
     <t xml:space="preserve">AgencyTypeID</t>
   </si>
   <si>
@@ -103,6 +124,18 @@
     <t xml:space="preserve">AgencyType 5</t>
   </si>
   <si>
+    <t xml:space="preserve">AgencyType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgencyType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgencyType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgencyType 9</t>
+  </si>
+  <si>
     <t xml:space="preserve">AssessmentCategoryTypeID</t>
   </si>
   <si>
@@ -115,21 +148,6 @@
     <t xml:space="preserve">AssessmentCategoryType 2</t>
   </si>
   <si>
-    <t xml:space="preserve">AssessmentCategoryType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AssessmentCategoryType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AssessmentCategoryType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AssessmentCategoryType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AssessmentCategoryType 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">BedTypeID</t>
   </si>
   <si>
@@ -139,15 +157,6 @@
     <t xml:space="preserve">BedType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">BedType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BedType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BedType 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">BehavioralHealthDiagnosisTypeID</t>
   </si>
   <si>
@@ -169,15 +178,6 @@
     <t xml:space="preserve">BehavioralHealthDiagnosisType 5</t>
   </si>
   <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisType 8</t>
-  </si>
-  <si>
     <t xml:space="preserve">BondStatusTypeID</t>
   </si>
   <si>
@@ -187,6 +187,9 @@
     <t xml:space="preserve">BondStatusType 1</t>
   </si>
   <si>
+    <t xml:space="preserve">BondStatusType 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">BondTypeID</t>
   </si>
   <si>
@@ -202,6 +205,27 @@
     <t xml:space="preserve">BondType 3</t>
   </si>
   <si>
+    <t xml:space="preserve">BondType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondType 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">CaseStatusTypeID</t>
   </si>
   <si>
@@ -238,6 +262,12 @@
     <t xml:space="preserve">CaseStatusType 10</t>
   </si>
   <si>
+    <t xml:space="preserve">CaseStatusType 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaseStatusType 12</t>
+  </si>
+  <si>
     <t xml:space="preserve">ChargeClassTypeID</t>
   </si>
   <si>
@@ -256,6 +286,24 @@
     <t xml:space="preserve">ChargeClassType 4</t>
   </si>
   <si>
+    <t xml:space="preserve">ChargeClassType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">ChargeTypeID</t>
   </si>
   <si>
@@ -265,6 +313,33 @@
     <t xml:space="preserve">ChargeType 1</t>
   </si>
   <si>
+    <t xml:space="preserve">ChargeType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeType 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">DomicileStatusTypeID</t>
   </si>
   <si>
@@ -280,6 +355,33 @@
     <t xml:space="preserve">DomicileStatusType 3</t>
   </si>
   <si>
+    <t xml:space="preserve">DomicileStatusType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomicileStatusType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomicileStatusType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomicileStatusType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomicileStatusType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomicileStatusType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomicileStatusType 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomicileStatusType 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomicileStatusType 12</t>
+  </si>
+  <si>
     <t xml:space="preserve">EducationLevelTypeID</t>
   </si>
   <si>
@@ -295,30 +397,6 @@
     <t xml:space="preserve">EducationLevelType 3</t>
   </si>
   <si>
-    <t xml:space="preserve">EducationLevelType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EducationLevelType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EducationLevelType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EducationLevelType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EducationLevelType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EducationLevelType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EducationLevelType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EducationLevelType 11</t>
-  </si>
-  <si>
     <t xml:space="preserve">JurisdictionTypeID</t>
   </si>
   <si>
@@ -346,12 +424,6 @@
     <t xml:space="preserve">JurisdictionType 7</t>
   </si>
   <si>
-    <t xml:space="preserve">JurisdictionType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JurisdictionType 9</t>
-  </si>
-  <si>
     <t xml:space="preserve">LanguageTypeID</t>
   </si>
   <si>
@@ -364,6 +436,27 @@
     <t xml:space="preserve">LanguageType 2</t>
   </si>
   <si>
+    <t xml:space="preserve">LanguageType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LanguageType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LanguageType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LanguageType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LanguageType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LanguageType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LanguageType 9</t>
+  </si>
+  <si>
     <t xml:space="preserve">MedicaidStatusTypeID</t>
   </si>
   <si>
@@ -394,6 +487,15 @@
     <t xml:space="preserve">MedicaidStatusType 8</t>
   </si>
   <si>
+    <t xml:space="preserve">MedicaidStatusType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicaidStatusType 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicaidStatusType 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">MedicationTypeID</t>
   </si>
   <si>
@@ -403,10 +505,28 @@
     <t xml:space="preserve">MedicationTypeDescription</t>
   </si>
   <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationType 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">V</t>
   </si>
   <si>
-    <t xml:space="preserve">MedicationType 1</t>
+    <t xml:space="preserve">MedicationType 4</t>
   </si>
   <si>
     <t xml:space="preserve">MilitaryServiceStatusTypeID</t>
@@ -424,24 +544,6 @@
     <t xml:space="preserve">MilitaryServiceStatusType 3</t>
   </si>
   <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 9</t>
-  </si>
-  <si>
     <t xml:space="preserve">OccupationTypeID</t>
   </si>
   <si>
@@ -457,9 +559,6 @@
     <t xml:space="preserve">OccupationType 3</t>
   </si>
   <si>
-    <t xml:space="preserve">OccupationType 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">PersonEthnicityTypeID</t>
   </si>
   <si>
@@ -475,6 +574,30 @@
     <t xml:space="preserve">PersonEthnicityType 3</t>
   </si>
   <si>
+    <t xml:space="preserve">PersonEthnicityType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">PersonRaceTypeID</t>
   </si>
   <si>
@@ -484,9 +607,6 @@
     <t xml:space="preserve">PersonRaceType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">PersonRaceType 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">PersonSexTypeID</t>
   </si>
   <si>
@@ -496,6 +616,9 @@
     <t xml:space="preserve">PersonSexType 1</t>
   </si>
   <si>
+    <t xml:space="preserve">PersonSexType 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">ProgramEligibilityTypeID</t>
   </si>
   <si>
@@ -517,21 +640,6 @@
     <t xml:space="preserve">ProgramEligibilityType 5</t>
   </si>
   <si>
-    <t xml:space="preserve">ProgramEligibilityType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgramEligibilityType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgramEligibilityType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgramEligibilityType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgramEligibilityType 10</t>
-  </si>
-  <si>
     <t xml:space="preserve">SexOffenderStatusTypeID</t>
   </si>
   <si>
@@ -541,13 +649,37 @@
     <t xml:space="preserve">SexOffenderStatusType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">TreatmentInitiationTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentInitiationTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentInitiationType 1</t>
+    <t xml:space="preserve">SexOffenderStatusType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SexOffenderStatusType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonTypeDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonType 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonType 7</t>
   </si>
   <si>
     <t xml:space="preserve">TreatmentStatusTypeID</t>
@@ -580,6 +712,15 @@
     <t xml:space="preserve">TreatmentStatusType 8</t>
   </si>
   <si>
+    <t xml:space="preserve">TreatmentStatusType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentStatusType 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentStatusType 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">WorkReleaseStatusTypeID</t>
   </si>
   <si>
@@ -605,12 +746,6 @@
   </si>
   <si>
     <t xml:space="preserve">WorkReleaseStatusType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkReleaseStatusType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkReleaseStatusType 9</t>
   </si>
 </sst>
 </file>
@@ -966,7 +1101,40 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -989,10 +1157,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
@@ -1000,7 +1168,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
@@ -1008,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
@@ -1016,7 +1184,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
@@ -1024,7 +1192,55 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1047,10 +1263,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
@@ -1058,7 +1274,79 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1081,10 +1369,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2">
@@ -1092,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3">
@@ -1100,7 +1388,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4">
@@ -1108,7 +1396,79 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1131,10 +1491,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -1142,7 +1502,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3">
@@ -1150,7 +1510,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4">
@@ -1158,71 +1518,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1245,10 +1541,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
@@ -1256,7 +1552,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3">
@@ -1264,7 +1560,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4">
@@ -1272,7 +1568,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5">
@@ -1280,7 +1576,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
@@ -1288,7 +1584,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7">
@@ -1296,7 +1592,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8">
@@ -1304,23 +1600,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1343,10 +1623,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2">
@@ -1354,7 +1634,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3">
@@ -1362,7 +1642,63 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1385,10 +1721,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
@@ -1396,7 +1732,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3">
@@ -1404,7 +1740,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4">
@@ -1412,7 +1748,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5">
@@ -1420,7 +1756,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6">
@@ -1428,7 +1764,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7">
@@ -1436,7 +1772,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8">
@@ -1444,7 +1780,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9">
@@ -1452,7 +1788,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1476,13 +1836,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2">
@@ -1490,10 +1850,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1516,10 +1909,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2">
@@ -1527,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
@@ -1535,7 +1928,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4">
@@ -1543,55 +1936,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1614,10 +1959,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2">
@@ -1625,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3">
@@ -1633,7 +1978,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4">
@@ -1641,15 +1986,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1672,10 +2009,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
@@ -1683,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -1691,7 +2028,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -1699,7 +2036,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -1707,7 +2044,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -1715,7 +2052,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -1723,7 +2060,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -1731,7 +2068,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -1739,7 +2076,39 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1762,10 +2131,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2">
@@ -1773,7 +2142,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
@@ -1781,7 +2150,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4">
@@ -1789,7 +2158,71 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1812,10 +2245,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2">
@@ -1823,15 +2256,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1854,10 +2279,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2">
@@ -1865,7 +2290,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1888,10 +2321,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2">
@@ -1899,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3">
@@ -1907,7 +2340,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4">
@@ -1915,7 +2348,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5">
@@ -1923,7 +2356,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6">
@@ -1931,47 +2364,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1994,10 +2387,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2">
@@ -2005,7 +2398,23 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2022,16 +2431,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="25.71" customWidth="1"/>
-    <col min="2" max="2" width="34.71" customWidth="1"/>
+    <col min="1" max="1" width="30.71" customWidth="1"/>
+    <col min="2" max="2" width="39.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2">
@@ -2039,7 +2448,55 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2062,10 +2519,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>214</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2">
@@ -2073,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3">
@@ -2081,7 +2538,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4">
@@ -2089,7 +2546,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5">
@@ -2097,7 +2554,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6">
@@ -2105,7 +2562,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7">
@@ -2113,7 +2570,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8">
@@ -2121,7 +2578,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9">
@@ -2129,7 +2586,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2152,10 +2633,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>227</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2">
@@ -2163,7 +2644,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
@@ -2171,7 +2652,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4">
@@ -2179,7 +2660,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5">
@@ -2187,7 +2668,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6">
@@ -2195,7 +2676,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7">
@@ -2203,7 +2684,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8">
@@ -2211,23 +2692,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>190</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2250,10 +2715,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
@@ -2261,7 +2726,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -2269,7 +2734,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -2277,7 +2742,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -2285,7 +2750,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -2293,7 +2758,39 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2316,10 +2813,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
@@ -2327,7 +2824,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -2335,47 +2832,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2398,10 +2855,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
@@ -2409,31 +2866,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2456,10 +2889,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
@@ -2467,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3">
@@ -2475,7 +2908,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
@@ -2483,7 +2916,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5">
@@ -2491,7 +2924,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6">
@@ -2499,30 +2932,6 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2560,6 +2969,14 @@
         <v>48</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2580,10 +2997,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2">
@@ -2591,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
@@ -2599,7 +3016,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -2607,7 +3024,63 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2630,10 +3103,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -2641,7 +3114,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -2649,7 +3122,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
@@ -2657,7 +3130,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
@@ -2665,7 +3138,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
@@ -2673,7 +3146,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
@@ -2681,7 +3154,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
@@ -2689,7 +3162,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
@@ -2697,7 +3170,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10">
@@ -2705,7 +3178,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
@@ -2713,7 +3186,23 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete demo staging load, except for prescribed medication (waiting on Cenpatico input)
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
@@ -7,38 +7,35 @@
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="EnrolledHealthcareProvider" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="AgencyType" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="AssessmentCategoryType" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="BedType" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="BehavioralHealthDiagnosisType" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="BondStatusType" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="BondType" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="CaseStatusType" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="ChargeClassType" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="ChargeType" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="DomicileStatusType" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="EducationLevelType" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="JurisdictionType" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="LanguageType" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="MedicaidStatusType" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="MedicationType" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="MilitaryServiceStatusType" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="OccupationType" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="PersonEthnicityType" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="PersonRaceType" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="PersonSexType" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="ProgramEligibilityType" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="SexOffenderStatusType" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="TreatmentAdmissionReasonType" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="TreatmentStatusType" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="WorkReleaseStatusType" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Agency" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="AssessmentCategoryType" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="BondStatusType" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="BondType" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="CaseStatusType" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ChargeClassType" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="DomicileStatusType" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="EducationLevelType" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="JurisdictionType" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="LanguageType" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="MedicaidStatusType" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="MedicationType" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="MilitaryServiceStatusType" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="OccupationType" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="PersonEthnicityType" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="PersonRaceType" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="PersonSexType" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="ProgramEligibilityType" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="SexOffenderStatusType" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="SupervisionUnitType" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="TreatmentAdmissionReasonType" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="TreatmentStatusType" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="WorkReleaseStatusType" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t xml:space="preserve">FacilityID</t>
   </si>
@@ -61,79 +58,19 @@
     <t xml:space="preserve">Facility 4</t>
   </si>
   <si>
-    <t xml:space="preserve">EnrolledHealthcareProviderID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProviderDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnrolledHealthcareProvider 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyType 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgencyType 9</t>
+    <t xml:space="preserve">Facility 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgencyID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgencyDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency 1</t>
   </si>
   <si>
     <t xml:space="preserve">AssessmentCategoryTypeID</t>
@@ -148,34 +85,19 @@
     <t xml:space="preserve">AssessmentCategoryType 2</t>
   </si>
   <si>
-    <t xml:space="preserve">BedTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BedTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BedType 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisType 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BehavioralHealthDiagnosisType 5</t>
+    <t xml:space="preserve">AssessmentCategoryType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssessmentCategoryType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssessmentCategoryType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssessmentCategoryType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssessmentCategoryType 7</t>
   </si>
   <si>
     <t xml:space="preserve">BondStatusTypeID</t>
@@ -190,6 +112,30 @@
     <t xml:space="preserve">BondStatusType 2</t>
   </si>
   <si>
+    <t xml:space="preserve">BondStatusType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondStatusType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondStatusType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondStatusType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondStatusType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondStatusType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondStatusType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondStatusType 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">BondTypeID</t>
   </si>
   <si>
@@ -211,21 +157,6 @@
     <t xml:space="preserve">BondType 5</t>
   </si>
   <si>
-    <t xml:space="preserve">BondType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 10</t>
-  </si>
-  <si>
     <t xml:space="preserve">CaseStatusTypeID</t>
   </si>
   <si>
@@ -247,27 +178,6 @@
     <t xml:space="preserve">CaseStatusType 5</t>
   </si>
   <si>
-    <t xml:space="preserve">CaseStatusType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseStatusType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseStatusType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseStatusType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseStatusType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseStatusType 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseStatusType 12</t>
-  </si>
-  <si>
     <t xml:space="preserve">ChargeClassTypeID</t>
   </si>
   <si>
@@ -277,69 +187,6 @@
     <t xml:space="preserve">ChargeClassType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">ChargeClassType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeClassType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeClassType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeClassType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeClassType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeClassType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeClassType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeClassType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeClassType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChargeType 10</t>
-  </si>
-  <si>
     <t xml:space="preserve">DomicileStatusTypeID</t>
   </si>
   <si>
@@ -397,6 +244,18 @@
     <t xml:space="preserve">EducationLevelType 3</t>
   </si>
   <si>
+    <t xml:space="preserve">EducationLevelType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EducationLevelType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EducationLevelType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EducationLevelType 7</t>
+  </si>
+  <si>
     <t xml:space="preserve">JurisdictionTypeID</t>
   </si>
   <si>
@@ -424,6 +283,12 @@
     <t xml:space="preserve">JurisdictionType 7</t>
   </si>
   <si>
+    <t xml:space="preserve">JurisdictionType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JurisdictionType 9</t>
+  </si>
+  <si>
     <t xml:space="preserve">LanguageTypeID</t>
   </si>
   <si>
@@ -457,6 +322,9 @@
     <t xml:space="preserve">LanguageType 9</t>
   </si>
   <si>
+    <t xml:space="preserve">LanguageType 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">MedicaidStatusTypeID</t>
   </si>
   <si>
@@ -496,6 +364,9 @@
     <t xml:space="preserve">MedicaidStatusType 11</t>
   </si>
   <si>
+    <t xml:space="preserve">MedicaidStatusType 12</t>
+  </si>
+  <si>
     <t xml:space="preserve">MedicationTypeID</t>
   </si>
   <si>
@@ -505,30 +376,12 @@
     <t xml:space="preserve">MedicationTypeDescription</t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
+    <t xml:space="preserve">T</t>
   </si>
   <si>
     <t xml:space="preserve">MedicationType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationType 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">MilitaryServiceStatusTypeID</t>
   </si>
   <si>
@@ -544,6 +397,12 @@
     <t xml:space="preserve">MilitaryServiceStatusType 3</t>
   </si>
   <si>
+    <t xml:space="preserve">MilitaryServiceStatusType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MilitaryServiceStatusType 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">OccupationTypeID</t>
   </si>
   <si>
@@ -559,6 +418,15 @@
     <t xml:space="preserve">OccupationType 3</t>
   </si>
   <si>
+    <t xml:space="preserve">OccupationType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OccupationType 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">PersonEthnicityTypeID</t>
   </si>
   <si>
@@ -568,36 +436,6 @@
     <t xml:space="preserve">PersonEthnicityType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">PersonEthnicityType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonEthnicityType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonEthnicityType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonEthnicityType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonEthnicityType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonEthnicityType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonEthnicityType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonEthnicityType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonEthnicityType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonEthnicityType 11</t>
-  </si>
-  <si>
     <t xml:space="preserve">PersonRaceTypeID</t>
   </si>
   <si>
@@ -607,6 +445,36 @@
     <t xml:space="preserve">PersonRaceType 1</t>
   </si>
   <si>
+    <t xml:space="preserve">PersonRaceType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonRaceType 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">PersonSexTypeID</t>
   </si>
   <si>
@@ -619,6 +487,30 @@
     <t xml:space="preserve">PersonSexType 2</t>
   </si>
   <si>
+    <t xml:space="preserve">PersonSexType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonSexType 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">ProgramEligibilityTypeID</t>
   </si>
   <si>
@@ -640,6 +532,9 @@
     <t xml:space="preserve">ProgramEligibilityType 5</t>
   </si>
   <si>
+    <t xml:space="preserve">ProgramEligibilityType 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">SexOffenderStatusTypeID</t>
   </si>
   <si>
@@ -655,6 +550,27 @@
     <t xml:space="preserve">SexOffenderStatusType 3</t>
   </si>
   <si>
+    <t xml:space="preserve">SexOffenderStatusType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitTypeDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitType 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitType 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">TreatmentAdmissionReasonTypeID</t>
   </si>
   <si>
@@ -679,9 +595,6 @@
     <t xml:space="preserve">TreatmentAdmissionReasonType 6</t>
   </si>
   <si>
-    <t xml:space="preserve">TreatmentAdmissionReasonType 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">TreatmentStatusTypeID</t>
   </si>
   <si>
@@ -691,36 +604,6 @@
     <t xml:space="preserve">TreatmentStatusType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">TreatmentStatusType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentStatusType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentStatusType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentStatusType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentStatusType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentStatusType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentStatusType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentStatusType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentStatusType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentStatusType 11</t>
-  </si>
-  <si>
     <t xml:space="preserve">WorkReleaseStatusTypeID</t>
   </si>
   <si>
@@ -740,12 +623,6 @@
   </si>
   <si>
     <t xml:space="preserve">WorkReleaseStatusType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkReleaseStatusType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkReleaseStatusType 7</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +978,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -1134,7 +1011,29 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1151,16 +1050,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="17.71" customWidth="1"/>
-    <col min="2" max="2" width="26.71" customWidth="1"/>
+    <col min="1" max="1" width="18.71" customWidth="1"/>
+    <col min="2" max="2" width="27.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
@@ -1168,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
@@ -1176,7 +1075,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
@@ -1184,7 +1083,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
@@ -1192,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6">
@@ -1200,7 +1099,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
@@ -1208,7 +1107,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
@@ -1216,7 +1115,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9">
@@ -1224,7 +1123,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
@@ -1232,15 +1131,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1257,16 +1148,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="12.71" customWidth="1"/>
-    <col min="2" max="2" width="21.71" customWidth="1"/>
+    <col min="1" max="1" width="14.71" customWidth="1"/>
+    <col min="2" max="2" width="23.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2">
@@ -1274,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3">
@@ -1282,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
@@ -1290,7 +1181,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
@@ -1298,7 +1189,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6">
@@ -1306,7 +1197,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7">
@@ -1314,7 +1205,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
@@ -1322,7 +1213,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
@@ -1330,7 +1221,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10">
@@ -1338,7 +1229,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11">
@@ -1346,7 +1237,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1369,10 +1260,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2">
@@ -1380,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
@@ -1388,7 +1279,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4">
@@ -1396,7 +1287,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -1404,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6">
@@ -1412,7 +1303,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7">
@@ -1420,7 +1311,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8">
@@ -1428,7 +1319,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
@@ -1436,7 +1327,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10">
@@ -1444,7 +1335,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
@@ -1452,7 +1343,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12">
@@ -1460,7 +1351,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13">
@@ -1468,7 +1359,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1485,16 +1376,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="20.71" customWidth="1"/>
-    <col min="2" max="2" width="29.71" customWidth="1"/>
+    <col min="1" max="1" width="16.71" customWidth="1"/>
+    <col min="2" max="2" width="28.71" customWidth="1"/>
+    <col min="3" max="3" width="25.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="2">
@@ -1502,23 +1397,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1535,16 +1417,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="18.71" customWidth="1"/>
-    <col min="2" max="2" width="27.71" customWidth="1"/>
+    <col min="1" max="1" width="27.71" customWidth="1"/>
+    <col min="2" max="2" width="36.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
@@ -1552,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3">
@@ -1560,7 +1442,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4">
@@ -1568,7 +1450,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5">
@@ -1576,7 +1458,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6">
@@ -1584,23 +1466,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1617,16 +1483,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="14.71" customWidth="1"/>
-    <col min="2" max="2" width="23.71" customWidth="1"/>
+    <col min="1" max="1" width="16.71" customWidth="1"/>
+    <col min="2" max="2" width="25.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2">
@@ -1634,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3">
@@ -1642,7 +1508,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4">
@@ -1650,7 +1516,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5">
@@ -1658,7 +1524,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6">
@@ -1666,7 +1532,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7">
@@ -1674,31 +1540,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1715,16 +1557,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="20.71" customWidth="1"/>
-    <col min="2" max="2" width="29.71" customWidth="1"/>
+    <col min="1" max="1" width="21.71" customWidth="1"/>
+    <col min="2" max="2" width="30.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2">
@@ -1732,87 +1574,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1830,19 +1592,15 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="16.71" customWidth="1"/>
-    <col min="2" max="2" width="28.71" customWidth="1"/>
-    <col min="3" max="3" width="25.71" customWidth="1"/>
+    <col min="2" max="2" width="25.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2">
@@ -1850,10 +1608,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3">
@@ -1861,10 +1616,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4">
@@ -1872,10 +1624,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5">
@@ -1883,10 +1632,63 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" t="s">
-        <v>162</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1903,16 +1705,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="27.71" customWidth="1"/>
-    <col min="2" max="2" width="36.71" customWidth="1"/>
+    <col min="1" max="1" width="15.71" customWidth="1"/>
+    <col min="2" max="2" width="24.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2">
@@ -1920,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3">
@@ -1928,7 +1730,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4">
@@ -1936,7 +1738,63 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1953,16 +1811,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.71" customWidth="1"/>
-    <col min="2" max="2" width="25.71" customWidth="1"/>
+    <col min="1" max="1" width="24.71" customWidth="1"/>
+    <col min="2" max="2" width="33.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2">
@@ -1970,7 +1828,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3">
@@ -1978,7 +1836,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4">
@@ -1986,7 +1844,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2003,16 +1885,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="28.71" customWidth="1"/>
-    <col min="2" max="2" width="37.71" customWidth="1"/>
+    <col min="1" max="1" width="8.71" customWidth="1"/>
+    <col min="2" max="2" width="17.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -2020,95 +1902,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2125,16 +1919,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.71" customWidth="1"/>
-    <col min="2" max="2" width="30.71" customWidth="1"/>
+    <col min="1" max="1" width="23.71" customWidth="1"/>
+    <col min="2" max="2" width="32.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2">
@@ -2142,7 +1936,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3">
@@ -2150,7 +1944,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4">
@@ -2158,7 +1952,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5">
@@ -2166,63 +1960,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2239,16 +1977,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.71" customWidth="1"/>
-    <col min="2" max="2" width="25.71" customWidth="1"/>
+    <col min="1" max="1" width="21.71" customWidth="1"/>
+    <col min="2" max="2" width="30.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2">
@@ -2256,7 +1994,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2273,16 +2035,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="15.71" customWidth="1"/>
-    <col min="2" max="2" width="24.71" customWidth="1"/>
+    <col min="1" max="1" width="30.71" customWidth="1"/>
+    <col min="2" max="2" width="39.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2">
@@ -2290,7 +2052,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3">
@@ -2298,7 +2060,39 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2315,16 +2109,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="24.71" customWidth="1"/>
-    <col min="2" max="2" width="33.71" customWidth="1"/>
+    <col min="1" max="1" width="21.71" customWidth="1"/>
+    <col min="2" max="2" width="30.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2">
@@ -2332,39 +2126,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2387,10 +2149,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2">
@@ -2398,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3">
@@ -2406,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4">
@@ -2414,57 +2176,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.71" customWidth="1"/>
-    <col min="2" max="2" width="39.71" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5">
@@ -2472,7 +2184,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6">
@@ -2480,219 +2192,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="21.71" customWidth="1"/>
-    <col min="2" max="2" width="30.71" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="23.71" customWidth="1"/>
-    <col min="2" max="2" width="32.71" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2709,16 +2209,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="12.71" customWidth="1"/>
-    <col min="2" max="2" width="21.71" customWidth="1"/>
+    <col min="1" max="1" width="24.71" customWidth="1"/>
+    <col min="2" max="2" width="33.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
@@ -2726,7 +2226,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -2734,7 +2234,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -2742,7 +2242,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -2750,7 +2250,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -2758,7 +2258,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -2766,7 +2266,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -2774,23 +2274,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2807,16 +2291,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="24.71" customWidth="1"/>
-    <col min="2" max="2" width="33.71" customWidth="1"/>
+    <col min="1" max="1" width="16.71" customWidth="1"/>
+    <col min="2" max="2" width="25.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
@@ -2824,7 +2308,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -2832,7 +2316,71 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2849,16 +2397,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="9.71" customWidth="1"/>
-    <col min="2" max="2" width="18.71" customWidth="1"/>
+    <col min="1" max="1" width="10.71" customWidth="1"/>
+    <col min="2" max="2" width="19.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
@@ -2866,7 +2414,39 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2883,16 +2463,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.71" customWidth="1"/>
-    <col min="2" max="2" width="40.71" customWidth="1"/>
+    <col min="1" max="1" width="16.71" customWidth="1"/>
+    <col min="2" max="2" width="25.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -2900,7 +2480,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
@@ -2908,7 +2488,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
@@ -2916,7 +2496,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -2924,7 +2504,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -2932,7 +2512,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2949,16 +2529,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.71" customWidth="1"/>
-    <col min="2" max="2" width="25.71" customWidth="1"/>
+    <col min="1" max="1" width="17.71" customWidth="1"/>
+    <col min="2" max="2" width="26.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
@@ -2966,14 +2546,6 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2991,8 +2563,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.71" customWidth="1"/>
-    <col min="2" max="2" width="19.71" customWidth="1"/>
+    <col min="1" max="1" width="20.71" customWidth="1"/>
+    <col min="2" max="2" width="29.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3081,6 +2653,22 @@
       </c>
       <c r="B11" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3097,16 +2685,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.71" customWidth="1"/>
-    <col min="2" max="2" width="25.71" customWidth="1"/>
+    <col min="1" max="1" width="20.71" customWidth="1"/>
+    <col min="2" max="2" width="29.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2">
@@ -3114,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
@@ -3122,7 +2710,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
@@ -3130,7 +2718,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
@@ -3138,7 +2726,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
@@ -3146,7 +2734,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
@@ -3154,7 +2742,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -3162,47 +2750,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished implementation of demo staging load
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
@@ -18,24 +18,23 @@
     <sheet name="JurisdictionType" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="LanguageType" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="MedicaidStatusType" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="MedicationType" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="MilitaryServiceStatusType" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="OccupationType" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="PersonEthnicityType" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="PersonRaceType" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="PersonSexType" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="ProgramEligibilityType" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="SexOffenderStatusType" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="SupervisionUnitType" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="TreatmentAdmissionReasonType" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="TreatmentStatusType" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="WorkReleaseStatusType" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="MilitaryServiceStatusType" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="OccupationType" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="PersonEthnicityType" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="PersonRaceType" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="PersonSexType" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="ProgramEligibilityType" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="SexOffenderStatusType" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="SupervisionUnitType" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="TreatmentAdmissionReasonType" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="TreatmentStatusType" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="WorkReleaseStatusType" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t xml:space="preserve">FacilityID</t>
   </si>
@@ -49,21 +48,6 @@
     <t xml:space="preserve">Facility 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Facility 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facility 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facility 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facility 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facility 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">AgencyID</t>
   </si>
   <si>
@@ -73,6 +57,30 @@
     <t xml:space="preserve">Agency 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Agency 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency 9</t>
+  </si>
+  <si>
     <t xml:space="preserve">AssessmentCategoryTypeID</t>
   </si>
   <si>
@@ -82,24 +90,6 @@
     <t xml:space="preserve">AssessmentCategoryType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">AssessmentCategoryType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AssessmentCategoryType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AssessmentCategoryType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AssessmentCategoryType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AssessmentCategoryType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AssessmentCategoryType 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">BondStatusTypeID</t>
   </si>
   <si>
@@ -121,21 +111,6 @@
     <t xml:space="preserve">BondStatusType 5</t>
   </si>
   <si>
-    <t xml:space="preserve">BondStatusType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondStatusType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondStatusType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondStatusType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondStatusType 10</t>
-  </si>
-  <si>
     <t xml:space="preserve">BondTypeID</t>
   </si>
   <si>
@@ -145,18 +120,6 @@
     <t xml:space="preserve">BondType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">BondType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BondType 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">CaseStatusTypeID</t>
   </si>
   <si>
@@ -172,12 +135,6 @@
     <t xml:space="preserve">CaseStatusType 3</t>
   </si>
   <si>
-    <t xml:space="preserve">CaseStatusType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseStatusType 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">ChargeClassTypeID</t>
   </si>
   <si>
@@ -187,6 +144,24 @@
     <t xml:space="preserve">ChargeClassType 1</t>
   </si>
   <si>
+    <t xml:space="preserve">ChargeClassType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChargeClassType 7</t>
+  </si>
+  <si>
     <t xml:space="preserve">DomicileStatusTypeID</t>
   </si>
   <si>
@@ -226,9 +201,6 @@
     <t xml:space="preserve">DomicileStatusType 11</t>
   </si>
   <si>
-    <t xml:space="preserve">DomicileStatusType 12</t>
-  </si>
-  <si>
     <t xml:space="preserve">EducationLevelTypeID</t>
   </si>
   <si>
@@ -250,12 +222,6 @@
     <t xml:space="preserve">EducationLevelType 5</t>
   </si>
   <si>
-    <t xml:space="preserve">EducationLevelType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EducationLevelType 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">JurisdictionTypeID</t>
   </si>
   <si>
@@ -289,6 +255,15 @@
     <t xml:space="preserve">JurisdictionType 9</t>
   </si>
   <si>
+    <t xml:space="preserve">JurisdictionType 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JurisdictionType 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JurisdictionType 12</t>
+  </si>
+  <si>
     <t xml:space="preserve">LanguageTypeID</t>
   </si>
   <si>
@@ -319,12 +294,6 @@
     <t xml:space="preserve">LanguageType 8</t>
   </si>
   <si>
-    <t xml:space="preserve">LanguageType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LanguageType 10</t>
-  </si>
-  <si>
     <t xml:space="preserve">MedicaidStatusTypeID</t>
   </si>
   <si>
@@ -367,21 +336,6 @@
     <t xml:space="preserve">MedicaidStatusType 12</t>
   </si>
   <si>
-    <t xml:space="preserve">MedicationTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GenericProductIdentification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationTypeDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationType 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">MilitaryServiceStatusTypeID</t>
   </si>
   <si>
@@ -391,18 +345,6 @@
     <t xml:space="preserve">MilitaryServiceStatusType 1</t>
   </si>
   <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MilitaryServiceStatusType 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">OccupationTypeID</t>
   </si>
   <si>
@@ -436,6 +378,18 @@
     <t xml:space="preserve">PersonEthnicityType 1</t>
   </si>
   <si>
+    <t xml:space="preserve">PersonEthnicityType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonEthnicityType 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">PersonRaceTypeID</t>
   </si>
   <si>
@@ -454,27 +408,6 @@
     <t xml:space="preserve">PersonRaceType 4</t>
   </si>
   <si>
-    <t xml:space="preserve">PersonRaceType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonRaceType 11</t>
-  </si>
-  <si>
     <t xml:space="preserve">PersonSexTypeID</t>
   </si>
   <si>
@@ -496,21 +429,6 @@
     <t xml:space="preserve">PersonSexType 5</t>
   </si>
   <si>
-    <t xml:space="preserve">PersonSexType 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PersonSexType 10</t>
-  </si>
-  <si>
     <t xml:space="preserve">ProgramEligibilityTypeID</t>
   </si>
   <si>
@@ -526,15 +444,6 @@
     <t xml:space="preserve">ProgramEligibilityType 3</t>
   </si>
   <si>
-    <t xml:space="preserve">ProgramEligibilityType 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgramEligibilityType 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgramEligibilityType 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">SexOffenderStatusTypeID</t>
   </si>
   <si>
@@ -553,6 +462,24 @@
     <t xml:space="preserve">SexOffenderStatusType 4</t>
   </si>
   <si>
+    <t xml:space="preserve">SexOffenderStatusType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SexOffenderStatusType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SexOffenderStatusType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SexOffenderStatusType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SexOffenderStatusType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SexOffenderStatusType 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">SupervisionUnitTypeID</t>
   </si>
   <si>
@@ -571,6 +498,24 @@
     <t xml:space="preserve">SupervisionUnitType 4</t>
   </si>
   <si>
+    <t xml:space="preserve">SupervisionUnitType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitType 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupervisionUnitType 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">TreatmentAdmissionReasonTypeID</t>
   </si>
   <si>
@@ -595,6 +540,9 @@
     <t xml:space="preserve">TreatmentAdmissionReasonType 6</t>
   </si>
   <si>
+    <t xml:space="preserve">TreatmentAdmissionReasonType 7</t>
+  </si>
+  <si>
     <t xml:space="preserve">TreatmentStatusTypeID</t>
   </si>
   <si>
@@ -604,6 +552,30 @@
     <t xml:space="preserve">TreatmentStatusType 1</t>
   </si>
   <si>
+    <t xml:space="preserve">TreatmentStatusType 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentStatusType 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentStatusType 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentStatusType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentStatusType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentStatusType 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentStatusType 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentStatusType 9</t>
+  </si>
+  <si>
     <t xml:space="preserve">WorkReleaseStatusTypeID</t>
   </si>
   <si>
@@ -623,6 +595,12 @@
   </si>
   <si>
     <t xml:space="preserve">WorkReleaseStatusType 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WorkReleaseStatusType 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WorkReleaseStatusType 7</t>
   </si>
 </sst>
 </file>
@@ -978,62 +956,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1056,10 +979,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -1067,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -1075,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
@@ -1083,7 +1006,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
@@ -1091,7 +1014,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
@@ -1099,7 +1022,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
@@ -1107,7 +1030,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
@@ -1115,7 +1038,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
@@ -1123,7 +1046,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10">
@@ -1131,7 +1054,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1154,10 +1101,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
@@ -1165,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
@@ -1173,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
@@ -1181,7 +1128,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
@@ -1189,7 +1136,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6">
@@ -1197,7 +1144,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7">
@@ -1205,7 +1152,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8">
@@ -1213,7 +1160,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
@@ -1221,23 +1168,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1260,10 +1191,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
@@ -1271,7 +1202,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
@@ -1279,7 +1210,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
@@ -1287,7 +1218,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
@@ -1295,7 +1226,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6">
@@ -1303,7 +1234,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
@@ -1311,7 +1242,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
@@ -1319,7 +1250,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
@@ -1327,7 +1258,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
@@ -1335,7 +1266,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
@@ -1343,7 +1274,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12">
@@ -1351,7 +1282,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13">
@@ -1359,7 +1290,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1376,20 +1307,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.71" customWidth="1"/>
-    <col min="2" max="2" width="28.71" customWidth="1"/>
-    <col min="3" max="3" width="25.71" customWidth="1"/>
+    <col min="1" max="1" width="27.71" customWidth="1"/>
+    <col min="2" max="2" width="36.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2">
@@ -1397,10 +1324,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1417,16 +1341,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="27.71" customWidth="1"/>
-    <col min="2" max="2" width="36.71" customWidth="1"/>
+    <col min="1" max="1" width="16.71" customWidth="1"/>
+    <col min="2" max="2" width="25.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
@@ -1434,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
@@ -1442,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
@@ -1450,7 +1374,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5">
@@ -1458,7 +1382,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
@@ -1466,7 +1390,15 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1483,16 +1415,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.71" customWidth="1"/>
-    <col min="2" max="2" width="25.71" customWidth="1"/>
+    <col min="1" max="1" width="21.71" customWidth="1"/>
+    <col min="2" max="2" width="30.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
@@ -1500,7 +1432,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3">
@@ -1508,7 +1440,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4">
@@ -1516,7 +1448,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5">
@@ -1524,7 +1456,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6">
@@ -1532,15 +1464,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1557,16 +1481,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.71" customWidth="1"/>
-    <col min="2" max="2" width="30.71" customWidth="1"/>
+    <col min="1" max="1" width="16.71" customWidth="1"/>
+    <col min="2" max="2" width="25.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2">
@@ -1574,7 +1498,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1591,16 +1539,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.71" customWidth="1"/>
-    <col min="2" max="2" width="25.71" customWidth="1"/>
+    <col min="1" max="1" width="15.71" customWidth="1"/>
+    <col min="2" max="2" width="24.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2">
@@ -1608,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
@@ -1616,7 +1564,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4">
@@ -1624,7 +1572,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
@@ -1632,7 +1580,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6">
@@ -1640,55 +1588,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1705,16 +1605,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="15.71" customWidth="1"/>
-    <col min="2" max="2" width="24.71" customWidth="1"/>
+    <col min="1" max="1" width="24.71" customWidth="1"/>
+    <col min="2" max="2" width="33.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2">
@@ -1722,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3">
@@ -1730,7 +1630,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4">
@@ -1738,63 +1638,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1811,16 +1655,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="24.71" customWidth="1"/>
-    <col min="2" max="2" width="33.71" customWidth="1"/>
+    <col min="1" max="1" width="23.71" customWidth="1"/>
+    <col min="2" max="2" width="32.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
@@ -1828,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3">
@@ -1836,7 +1680,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4">
@@ -1844,7 +1688,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5">
@@ -1852,7 +1696,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6">
@@ -1860,7 +1704,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7">
@@ -1868,7 +1712,39 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1891,10 +1767,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -1902,7 +1778,71 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1919,16 +1859,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="23.71" customWidth="1"/>
-    <col min="2" max="2" width="32.71" customWidth="1"/>
+    <col min="1" max="1" width="21.71" customWidth="1"/>
+    <col min="2" max="2" width="30.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2">
@@ -1936,7 +1876,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3">
@@ -1944,7 +1884,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4">
@@ -1952,7 +1892,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5">
@@ -1960,7 +1900,55 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1977,16 +1965,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.71" customWidth="1"/>
-    <col min="2" max="2" width="30.71" customWidth="1"/>
+    <col min="1" max="1" width="30.71" customWidth="1"/>
+    <col min="2" max="2" width="39.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
@@ -1994,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3">
@@ -2002,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4">
@@ -2010,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5">
@@ -2018,7 +2006,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2035,16 +2047,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="30.71" customWidth="1"/>
-    <col min="2" max="2" width="39.71" customWidth="1"/>
+    <col min="1" max="1" width="21.71" customWidth="1"/>
+    <col min="2" max="2" width="30.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2">
@@ -2052,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3">
@@ -2060,7 +2072,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4">
@@ -2068,7 +2080,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5">
@@ -2076,7 +2088,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6">
@@ -2084,7 +2096,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7">
@@ -2092,7 +2104,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2109,50 +2145,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.71" customWidth="1"/>
-    <col min="2" max="2" width="30.71" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
     <col min="1" max="1" width="23.71" customWidth="1"/>
     <col min="2" max="2" width="32.71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2">
@@ -2160,7 +2162,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3">
@@ -2168,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4">
@@ -2176,7 +2178,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5">
@@ -2184,7 +2186,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6">
@@ -2192,7 +2194,23 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>195</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2215,10 +2233,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
@@ -2226,55 +2244,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2297,10 +2267,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -2308,7 +2278,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -2316,7 +2286,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
@@ -2324,7 +2294,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -2332,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -2340,47 +2310,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2403,10 +2333,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
@@ -2414,39 +2344,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2469,10 +2367,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
@@ -2480,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -2488,7 +2386,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
@@ -2496,23 +2394,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2535,10 +2417,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
@@ -2546,7 +2428,55 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2569,10 +2499,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">
@@ -2580,7 +2510,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -2588,7 +2518,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
@@ -2596,7 +2526,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
@@ -2604,7 +2534,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6">
@@ -2612,7 +2542,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
@@ -2620,7 +2550,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
@@ -2628,7 +2558,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9">
@@ -2636,7 +2566,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -2644,7 +2574,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11">
@@ -2652,7 +2582,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12">
@@ -2660,15 +2590,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2691,10 +2613,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2">
@@ -2702,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -2710,7 +2632,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
@@ -2718,7 +2640,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
@@ -2726,7 +2648,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
@@ -2734,23 +2656,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Drop the CaseStatusType code table and add BookingCharge.ChargeDisposition.
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="14260" firstSheet="17" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="14260" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="1" r:id="rId1"/>
@@ -12,22 +12,21 @@
     <sheet name="AssessmentCategoryType" sheetId="3" r:id="rId3"/>
     <sheet name="BondStatusType" sheetId="4" r:id="rId4"/>
     <sheet name="BondType" sheetId="5" r:id="rId5"/>
-    <sheet name="CaseStatusType" sheetId="6" r:id="rId6"/>
-    <sheet name="ChargeClassType" sheetId="7" r:id="rId7"/>
-    <sheet name="DomicileStatusType" sheetId="8" r:id="rId8"/>
-    <sheet name="JurisdictionType" sheetId="10" r:id="rId9"/>
-    <sheet name="LanguageType" sheetId="11" r:id="rId10"/>
-    <sheet name="MedicaidStatusType" sheetId="12" r:id="rId11"/>
-    <sheet name="MilitaryServiceStatusType" sheetId="13" r:id="rId12"/>
-    <sheet name="PersonEthnicityType" sheetId="15" r:id="rId13"/>
-    <sheet name="PersonRaceType" sheetId="16" r:id="rId14"/>
-    <sheet name="PersonSexType" sheetId="17" r:id="rId15"/>
-    <sheet name="ProgramEligibilityType" sheetId="18" r:id="rId16"/>
-    <sheet name="SexOffenderStatusType" sheetId="19" r:id="rId17"/>
-    <sheet name="SupervisionUnitType" sheetId="20" r:id="rId18"/>
-    <sheet name="TreatmentAdmissionReasonType" sheetId="21" r:id="rId19"/>
-    <sheet name="TreatmentStatusType" sheetId="22" r:id="rId20"/>
-    <sheet name="WorkReleaseStatusType" sheetId="23" r:id="rId21"/>
+    <sheet name="ChargeClassType" sheetId="7" r:id="rId6"/>
+    <sheet name="DomicileStatusType" sheetId="8" r:id="rId7"/>
+    <sheet name="JurisdictionType" sheetId="10" r:id="rId8"/>
+    <sheet name="LanguageType" sheetId="11" r:id="rId9"/>
+    <sheet name="MedicaidStatusType" sheetId="12" r:id="rId10"/>
+    <sheet name="MilitaryServiceStatusType" sheetId="13" r:id="rId11"/>
+    <sheet name="PersonEthnicityType" sheetId="15" r:id="rId12"/>
+    <sheet name="PersonRaceType" sheetId="16" r:id="rId13"/>
+    <sheet name="PersonSexType" sheetId="17" r:id="rId14"/>
+    <sheet name="ProgramEligibilityType" sheetId="18" r:id="rId15"/>
+    <sheet name="SexOffenderStatusType" sheetId="19" r:id="rId16"/>
+    <sheet name="SupervisionUnitType" sheetId="20" r:id="rId17"/>
+    <sheet name="TreatmentAdmissionReasonType" sheetId="21" r:id="rId18"/>
+    <sheet name="TreatmentStatusType" sheetId="22" r:id="rId19"/>
+    <sheet name="WorkReleaseStatusType" sheetId="23" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
   <si>
     <t>FacilityID</t>
   </si>
@@ -123,21 +122,6 @@
   </si>
   <si>
     <t>BondType 1</t>
-  </si>
-  <si>
-    <t>CaseStatusTypeID</t>
-  </si>
-  <si>
-    <t>CaseStatusTypeDescription</t>
-  </si>
-  <si>
-    <t>CaseStatusType 1</t>
-  </si>
-  <si>
-    <t>CaseStatusType 2</t>
-  </si>
-  <si>
-    <t>CaseStatusType 3</t>
   </si>
   <si>
     <t>ChargeClassTypeID</t>
@@ -932,22 +916,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -955,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -963,7 +947,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -971,7 +955,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -979,7 +963,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -987,7 +971,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -995,7 +979,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1003,7 +987,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1011,7 +995,39 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1027,22 +1043,22 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1050,95 +1066,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1154,22 +1082,22 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1177,7 +1105,39 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1193,22 +1153,22 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1216,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1224,7 +1184,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1232,7 +1192,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1240,15 +1200,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1264,22 +1216,22 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1287,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1295,7 +1247,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1303,7 +1255,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1311,7 +1263,15 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1327,22 +1287,22 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1350,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1358,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1366,22 +1326,6 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1398,14 +1342,14 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1438,6 +1382,62 @@
       </c>
       <c r="B4" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1459,16 +1459,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1484,7 +1484,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1492,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1500,7 +1500,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1508,7 +1508,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1516,7 +1516,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1524,7 +1524,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1532,7 +1532,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1540,7 +1540,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1548,7 +1548,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1564,22 +1564,22 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1587,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1595,7 +1595,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1603,7 +1603,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1611,7 +1611,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1619,7 +1619,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1627,7 +1627,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1635,31 +1635,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1675,22 +1651,22 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1698,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1706,7 +1682,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1714,7 +1690,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1722,7 +1698,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1730,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1738,7 +1714,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1746,7 +1722,23 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1865,109 +1857,6 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1980,10 +1869,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1991,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1999,7 +1888,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2007,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2015,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2023,7 +1912,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2031,7 +1920,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2039,7 +1928,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2204,14 +2093,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2244,6 +2133,38 @@
       </c>
       <c r="B4" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2259,22 +2180,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2282,7 +2203,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2290,7 +2211,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2298,7 +2219,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2306,7 +2227,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2314,7 +2235,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2322,7 +2243,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2330,7 +2251,39 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2346,22 +2299,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2369,7 +2322,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2377,7 +2330,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2385,7 +2338,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2393,7 +2346,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2401,7 +2354,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2409,7 +2362,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2417,7 +2370,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2425,7 +2378,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2433,7 +2386,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2441,7 +2394,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2449,7 +2402,15 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2465,22 +2426,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2488,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2496,7 +2457,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2504,7 +2465,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2512,7 +2473,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2520,7 +2481,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2528,7 +2489,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2536,7 +2497,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2544,39 +2505,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated universal code tables with more sensible values
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/StagingCodeTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="14260" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="14265" firstSheet="15" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="169">
   <si>
     <t>FacilityID</t>
   </si>
@@ -319,60 +319,18 @@
     <t>PersonEthnicityTypeDescription</t>
   </si>
   <si>
-    <t>PersonEthnicityType 1</t>
-  </si>
-  <si>
-    <t>PersonEthnicityType 2</t>
-  </si>
-  <si>
-    <t>PersonEthnicityType 3</t>
-  </si>
-  <si>
-    <t>PersonEthnicityType 4</t>
-  </si>
-  <si>
-    <t>PersonEthnicityType 5</t>
-  </si>
-  <si>
     <t>PersonRaceTypeID</t>
   </si>
   <si>
     <t>PersonRaceTypeDescription</t>
   </si>
   <si>
-    <t>PersonRaceType 1</t>
-  </si>
-  <si>
-    <t>PersonRaceType 2</t>
-  </si>
-  <si>
-    <t>PersonRaceType 3</t>
-  </si>
-  <si>
-    <t>PersonRaceType 4</t>
-  </si>
-  <si>
     <t>PersonSexTypeID</t>
   </si>
   <si>
     <t>PersonSexTypeDescription</t>
   </si>
   <si>
-    <t>PersonSexType 1</t>
-  </si>
-  <si>
-    <t>PersonSexType 2</t>
-  </si>
-  <si>
-    <t>PersonSexType 3</t>
-  </si>
-  <si>
-    <t>PersonSexType 4</t>
-  </si>
-  <si>
-    <t>PersonSexType 5</t>
-  </si>
-  <si>
     <t>ProgramEligibilityTypeID</t>
   </si>
   <si>
@@ -545,6 +503,48 @@
   </si>
   <si>
     <t>WorkReleaseStatusType 7</t>
+  </si>
+  <si>
+    <t>MilitaryServiceStatusType 2</t>
+  </si>
+  <si>
+    <t>MilitaryServiceStatusType 3</t>
+  </si>
+  <si>
+    <t>BondType 2</t>
+  </si>
+  <si>
+    <t>BondType 3</t>
+  </si>
+  <si>
+    <t>Non-Hispanic</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Black / African-American</t>
+  </si>
+  <si>
+    <t>American Indian / Alaska Native</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -588,6 +588,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -874,14 +879,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -920,13 +925,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -934,7 +939,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -942,7 +947,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -950,7 +955,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -958,7 +963,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -966,7 +971,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -974,7 +979,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -982,7 +987,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -990,7 +995,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -998,7 +1003,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1006,7 +1011,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1014,7 +1019,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1022,7 +1027,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1043,17 +1048,19 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -1061,12 +1068,28 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1082,17 +1105,19 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -1100,44 +1125,28 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1153,54 +1162,72 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1216,62 +1243,40 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1289,44 +1294,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1346,98 +1353,98 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1457,98 +1464,98 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1568,74 +1575,74 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1655,90 +1662,90 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1758,13 +1765,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1772,7 +1779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1780,7 +1787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1788,7 +1795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1796,7 +1803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1804,7 +1811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1812,7 +1819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1820,7 +1827,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1828,7 +1835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1836,7 +1843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1861,74 +1868,74 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1948,13 +1955,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1962,7 +1969,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1987,13 +1994,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2001,7 +2008,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2009,7 +2016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2017,7 +2024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2025,7 +2032,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2033,7 +2040,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2054,17 +2061,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2072,12 +2081,28 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2095,15 +2120,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2111,7 +2136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2119,7 +2144,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2127,7 +2152,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2135,7 +2160,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2143,7 +2168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2151,7 +2176,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2159,7 +2184,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2184,13 +2209,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -2198,7 +2223,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2206,7 +2231,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2214,7 +2239,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2222,7 +2247,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2230,7 +2255,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2238,7 +2263,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2246,7 +2271,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2254,7 +2279,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2262,7 +2287,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2270,7 +2295,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2278,7 +2303,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2303,13 +2328,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -2317,7 +2342,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2325,7 +2350,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2333,7 +2358,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2341,7 +2366,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2349,7 +2374,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2357,7 +2382,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2365,7 +2390,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2373,7 +2398,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2381,7 +2406,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2389,7 +2414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2397,7 +2422,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2405,7 +2430,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2430,13 +2455,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -2444,7 +2469,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2452,7 +2477,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2460,7 +2485,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2468,7 +2493,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2476,7 +2501,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2484,7 +2509,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2492,7 +2517,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2500,7 +2525,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>

</xml_diff>